<commit_message>
T2Dm complications at initiations assigned
DONE
1. Tidied up health states and daly weights
2. checked correct daly values are assigned
3. Generated properties for t2dm complications
4. Upload data on complications
5. Complications at t0 assigned

To Do:
1. Check complications prevalence against data
2. Try read in BMI csv Stef Excel read in (list)
3. flake8 redo on additional code
4. Upload Price data for t2dm and htn

Post UCl review
1. Trial outreach campaign
2. Trial HSI event
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_T2DM.xlsx
+++ b/resources/ResourceFile_Method_T2DM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60801664-D657-F847-8E56-2A5112C0B7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10D8BD7-93C2-3846-8D58-AD22213E5002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="141">
   <si>
     <t>Name:</t>
   </si>
@@ -505,6 +505,57 @@
   </si>
   <si>
     <t>prob_neurocomp</t>
+  </si>
+  <si>
+    <t>p_stroke</t>
+  </si>
+  <si>
+    <t>p_nephro_1</t>
+  </si>
+  <si>
+    <t>p_nephro_2</t>
+  </si>
+  <si>
+    <t>p_nephro_3</t>
+  </si>
+  <si>
+    <t>p_neuro_1</t>
+  </si>
+  <si>
+    <t>p_neuro_2</t>
+  </si>
+  <si>
+    <t>p_neuro_3</t>
+  </si>
+  <si>
+    <t>p_retino_1</t>
+  </si>
+  <si>
+    <t>p_retino_2</t>
+  </si>
+  <si>
+    <t>prob_nephro_1</t>
+  </si>
+  <si>
+    <t>prob_nephro_2</t>
+  </si>
+  <si>
+    <t>prob_nephro_3</t>
+  </si>
+  <si>
+    <t>prob_neuro_1</t>
+  </si>
+  <si>
+    <t>prob_neuro_2</t>
+  </si>
+  <si>
+    <t>prob_neuro_3</t>
+  </si>
+  <si>
+    <t>prob_retino_1</t>
+  </si>
+  <si>
+    <t>prob_retino_2</t>
   </si>
 </sst>
 </file>
@@ -767,7 +818,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -857,6 +908,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1690,7 +1743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C57" sqref="C57:C82"/>
     </sheetView>
   </sheetViews>
@@ -3661,29 +3714,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFD66BD-C60D-C14A-9E33-3479AADC1850}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="44"/>
+    <col min="2" max="4" width="10.83203125" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="52" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3691,13 +3744,13 @@
       <c r="A2" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="52">
         <v>1</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="52">
         <v>1</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="52">
         <v>1</v>
       </c>
     </row>
@@ -3705,13 +3758,13 @@
       <c r="A3" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="52">
         <v>1.49</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="52">
         <v>1.26</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="52">
         <v>1.77</v>
       </c>
     </row>
@@ -3719,13 +3772,13 @@
       <c r="A4" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="52">
         <v>1.58</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="52">
         <v>1.56</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="52">
         <v>1.59</v>
       </c>
     </row>
@@ -3733,13 +3786,13 @@
       <c r="A5" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="52">
         <v>1.57</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="52">
         <v>1.39</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="52">
         <v>1.8</v>
       </c>
     </row>
@@ -3747,7 +3800,7 @@
       <c r="A6" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="52">
         <v>0.35599999999999998</v>
       </c>
     </row>
@@ -3755,7 +3808,7 @@
       <c r="A7" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="52">
         <v>0.33100000000000002</v>
       </c>
     </row>
@@ -3763,7 +3816,7 @@
       <c r="A8" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="52">
         <v>0.32300000000000001</v>
       </c>
     </row>
@@ -3771,8 +3824,83 @@
       <c r="A9" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="52">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="52">
+        <f>0.366+B11</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="52">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="52">
+        <f>0.347+B13+B14</f>
+        <v>0.47809944751381217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="52">
+        <f>0.109+B14</f>
+        <v>0.12004972375690608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="52">
+        <f>2/181</f>
+        <v>1.1049723756906077E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="52">
+        <f>0.464+B16+B17</f>
+        <v>0.56400000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="52">
+        <f>0.06+B17</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="52">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3782,10 +3910,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1478562-9F3F-AD46-9C84-EECEDF46D70E}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:F8"/>
+      <selection activeCell="A18" sqref="A18:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4108,6 +4236,134 @@
       </c>
       <c r="F16">
         <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>90</v>
+      </c>
+      <c r="D17">
+        <f>35/478</f>
+        <v>7.3221757322175729E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>90</v>
+      </c>
+      <c r="D18">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>90</v>
+      </c>
+      <c r="D19">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>90</v>
+      </c>
+      <c r="D20">
+        <f>2/181</f>
+        <v>1.1049723756906077E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <v>0.46400000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>90</v>
+      </c>
+      <c r="D23">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>90</v>
+      </c>
+      <c r="D24">
+        <v>0.36599999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>90</v>
+      </c>
+      <c r="D25">
+        <v>7.3999999999999996E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prevalent T2DM complications assigned and tested.
DONE
1. Tidied up health states and daly weights
2. checked correct daly values are assigned
3. Generated properties for t2dm complications
4. Upload data on complications
5. Complications at t0 assigned
6. Check complications prevalence against data

To Do:
1. Add incident complications
2. Try read in BMI csv Stef Excel read in (list)
3. flake8 redo on additional code
4. Upload Price data for t2dm and htn

Post UCl review
1. Trial outreach campaign
2. Trial HSI event
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_T2DM.xlsx
+++ b/resources/ResourceFile_Method_T2DM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10D8BD7-93C2-3846-8D58-AD22213E5002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC5066-6580-754A-82CF-D1B87DF3CBE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="140">
   <si>
     <t>Name:</t>
   </si>
@@ -495,18 +495,9 @@
     <t>prob_d2givengd</t>
   </si>
   <si>
-    <t>prob_retinocomp</t>
-  </si>
-  <si>
-    <t>prob_nephrocomp</t>
-  </si>
-  <si>
     <t>prob_death</t>
   </si>
   <si>
-    <t>prob_neurocomp</t>
-  </si>
-  <si>
     <t>p_stroke</t>
   </si>
   <si>
@@ -516,53 +507,62 @@
     <t>p_nephro_2</t>
   </si>
   <si>
-    <t>p_nephro_3</t>
-  </si>
-  <si>
     <t>p_neuro_1</t>
   </si>
   <si>
     <t>p_neuro_2</t>
   </si>
   <si>
-    <t>p_neuro_3</t>
-  </si>
-  <si>
     <t>p_retino_1</t>
   </si>
   <si>
     <t>p_retino_2</t>
   </si>
   <si>
-    <t>prob_nephro_1</t>
-  </si>
-  <si>
-    <t>prob_nephro_2</t>
-  </si>
-  <si>
-    <t>prob_nephro_3</t>
-  </si>
-  <si>
-    <t>prob_neuro_1</t>
-  </si>
-  <si>
-    <t>prob_neuro_2</t>
-  </si>
-  <si>
-    <t>prob_neuro_3</t>
-  </si>
-  <si>
-    <t>prob_retino_1</t>
-  </si>
-  <si>
-    <t>prob_retino_2</t>
+    <t>prev_retino_1</t>
+  </si>
+  <si>
+    <t>prev_retino_2</t>
+  </si>
+  <si>
+    <t>prev_nephro_1</t>
+  </si>
+  <si>
+    <t>prev_nephro_2</t>
+  </si>
+  <si>
+    <t>prev_neuro_1</t>
+  </si>
+  <si>
+    <t>prev_neuro_2</t>
+  </si>
+  <si>
+    <t>prob_neurocomp_1</t>
+  </si>
+  <si>
+    <t>prob_neurocomp_2</t>
+  </si>
+  <si>
+    <t>prob_nephrocomp_1</t>
+  </si>
+  <si>
+    <t>prob_nephrocomp_2</t>
+  </si>
+  <si>
+    <t>prob_retinocomp_1</t>
+  </si>
+  <si>
+    <t>prob_retinocomp_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000000000"/>
+  </numFmts>
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -667,6 +667,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -818,7 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -910,6 +917,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3714,19 +3724,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFD66BD-C60D-C14A-9E33-3479AADC1850}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="43" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.83203125" style="52"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>117</v>
       </c>
@@ -3740,7 +3751,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
         <v>118</v>
       </c>
@@ -3754,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
         <v>116</v>
       </c>
@@ -3768,7 +3779,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
         <v>115</v>
       </c>
@@ -3782,7 +3793,7 @@
         <v>1.59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
         <v>119</v>
       </c>
@@ -3796,112 +3807,138 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="52">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="52">
+        <v>3.9600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="54">
+        <v>5.9799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="54">
+        <v>3.9199999999999999E-3</v>
+      </c>
+      <c r="C9" s="52">
+        <v>7.8030435827659839E-4</v>
+      </c>
+      <c r="D9" s="52">
+        <v>7.0648977221217189E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="54">
+        <f>AVERAGE(C10:D10)</f>
+        <v>7.4499999999999997E-2</v>
+      </c>
+      <c r="C10" s="52">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D10" s="52">
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="54">
+        <f>AVERAGE(C11:D11)</f>
+        <v>7.85E-2</v>
+      </c>
+      <c r="C11" s="52">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D11" s="52">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="52">
-        <v>0.35599999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="52">
-        <v>0.33100000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="52">
-        <v>0.32300000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="52">
+      <c r="B12" s="52">
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" s="52">
-        <f>0.366+B11</f>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="52">
-        <v>7.3999999999999996E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="51" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="52">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="52">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="52">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="B12" s="52">
-        <f>0.347+B13+B14</f>
-        <v>0.47809944751381217</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" s="52">
-        <f>0.109+B14</f>
-        <v>0.12004972375690608</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="52">
-        <f>2/181</f>
-        <v>1.1049723756906077E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="B15" s="52">
-        <f>0.464+B16+B17</f>
-        <v>0.56400000000000006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="51" t="s">
-        <v>137</v>
-      </c>
       <c r="B16" s="52">
-        <f>0.06+B17</f>
-        <v>0.08</v>
-      </c>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="51" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B17" s="52">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E22" t="s">
+        <v>0.35599999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="52">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
         <v>54</v>
       </c>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3910,10 +3947,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1478562-9F3F-AD46-9C84-EECEDF46D70E}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D25"/>
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4240,7 +4277,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -4255,7 +4292,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -4269,7 +4306,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4278,12 +4315,12 @@
         <v>90</v>
       </c>
       <c r="D19">
-        <v>0.109</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -4292,13 +4329,12 @@
         <v>90</v>
       </c>
       <c r="D20">
-        <f>2/181</f>
-        <v>1.1049723756906077E-2</v>
+        <v>0.32200000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B21">
         <v>18</v>
@@ -4307,12 +4343,12 @@
         <v>90</v>
       </c>
       <c r="D21">
-        <v>0.46400000000000002</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B22">
         <v>18</v>
@@ -4321,12 +4357,12 @@
         <v>90</v>
       </c>
       <c r="D22">
-        <v>0.06</v>
+        <v>0.35599999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B23">
         <v>18</v>
@@ -4335,35 +4371,7 @@
         <v>90</v>
       </c>
       <c r="D23">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B24">
-        <v>18</v>
-      </c>
-      <c r="C24">
-        <v>90</v>
-      </c>
-      <c r="D24">
-        <v>0.36599999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25">
-        <v>18</v>
-      </c>
-      <c r="C25">
-        <v>90</v>
-      </c>
-      <c r="D25">
-        <v>7.3999999999999996E-2</v>
+        <v>0.245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalise Diabetes event (incident complications and progression)
DONE
1. Tidied up health states and daly weights
2. checked correct daly values are assigned
3. Generated properties for t2dm complications
4. Upload data on complications
5. Complications at t0 assigned
6. Check complications prevalence against data

To Do:
1. Check complications against data
2. Try read in BMI csv Stef Excel read in (list)
3. flake8 redo on additional code
4. Upload Price data for t2dm and htn

Post UCl review
1. Trial outreach campaign
2. Trial HSI event
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_T2DM.xlsx
+++ b/resources/ResourceFile_Method_T2DM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC5066-6580-754A-82CF-D1B87DF3CBE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023D8A0A-6594-D143-925D-EBBA2935772C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26720" tabRatio="723" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34140" yWindow="460" windowWidth="17060" windowHeight="26720" tabRatio="723" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -3727,7 +3727,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Excel Resource file has been cleaned and updated
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Method_T2DM.xlsx
+++ b/resources/ResourceFile_Method_T2DM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc1405/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023D8A0A-6594-D143-925D-EBBA2935772C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87CEEFA-97B0-2D44-AFBE-0022E632A5F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34140" yWindow="460" windowWidth="17060" windowHeight="26720" tabRatio="723" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" tabRatio="723" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="141">
   <si>
     <t>Name:</t>
   </si>
@@ -122,12 +122,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>not currently but later: li_overwt; li_tob</t>
-  </si>
-  <si>
-    <t>sex, dateofbirth</t>
-  </si>
-  <si>
     <t>Lifestyle Elements requiered:</t>
   </si>
   <si>
@@ -164,13 +158,6 @@
     <t>see 'parameters'</t>
   </si>
   <si>
-    <t xml:space="preserve">
-diabetes_current_status (Diabetes module)</t>
-  </si>
-  <si>
-    <t>diabetes</t>
-  </si>
-  <si>
     <t>community-based screening, screen high risk (primary care), diabetes treatment &amp; interventions (community to referral hospital)</t>
   </si>
   <si>
@@ -189,30 +176,13 @@
     <t>probability</t>
   </si>
   <si>
-    <t>Cardiovascular disease, Hypertension, High cholesterol</t>
-  </si>
-  <si>
-    <t>Handle multiple risks</t>
-  </si>
-  <si>
     <t>Diagnosed</t>
   </si>
   <si>
-    <t>diab_risk (risk ratio)
-diab_current_status (yes; no)
-diab_historic_status (N=never; C=current; P=previous)
-diab_date_case (date of latest case)
-diab_treatment_status (N=never; C=current; P=previous)
-diab_date_treatment (date of latest treatment)</t>
-  </si>
-  <si>
     <t>Diagnosed with diabetes</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Incorpporate deaths</t>
   </si>
   <si>
     <t>Details of health service to be developed, including treatment (un)success; diagnosis and recovery)</t>
@@ -266,9 +236,6 @@
   </si>
   <si>
     <t>If treatment is stopped, person is assumed to have diabetes, unless sucessful lifestyle intervention</t>
-  </si>
-  <si>
-    <t>Prevalence/incidence to also depend on lifestyle factors and pre-existing conditions</t>
   </si>
   <si>
     <t>value</t>
@@ -554,13 +521,63 @@
   <si>
     <t>prob_retinocomp_2</t>
   </si>
+  <si>
+    <t>d2_age_range (age range for t2dm validation)
+d2_risk (risk ratio)
+d2_current_status (yes; no)
+d2_historic_status (N=never; C=current; P=previous)
+d2_date (date of t2dm)
+d2_nephro_date (date of latest nephropathy)
+d2_nephro_status (0=no, 1=mild, 2=severe)
+d2_neuro_date (date of latest neuropathy)
+d2_neuro_status (0=no, 1=mild, 2=severe)
+d2_retino_date (date of latest retinopathy)
+d2_retino_status (0=no, 1=mild, 2=severe)
+d2_death_date (date of death)
+d2_diag_date (date of latest diagnosis)
+d2_diag_status (yes; no)
+d2_treat_date (date of latest treatment)
+d2_treat_status (yes; no)
+d2_contr_date (date of latest control)
+d2_contr_status (yes; no)
+d2_specific_symptoms 
+d2_unified_symptoms_code</t>
+  </si>
+  <si>
+    <t>Cardiovascular disease, Hypertension,</t>
+  </si>
+  <si>
+    <t>li_bmi</t>
+  </si>
+  <si>
+    <t>sex, dateofbirth, mother_id, gestational_diabetes, hypertension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ht_current_status (Hypertension module), gd_current_status (Gestational diabetes module)</t>
+  </si>
+  <si>
+    <t>hypertension, gestational diabetes</t>
+  </si>
+  <si>
+    <t>In code change overweight to bmi</t>
+  </si>
+  <si>
+    <t>In code activate hypertension once circular definition has been addressed</t>
+  </si>
+  <si>
+    <t>In code add gestational diabetes as risk factor once method is developed</t>
+  </si>
+  <si>
+    <t>In code add mortality due to complicaitons</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -919,7 +936,7 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -943,29 +960,31 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>785091</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1535545</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1884218</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>23091</xdr:rowOff>
+      <xdr:rowOff>207162</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3036C6AC-6D7D-6C40-972B-8F1BCE8F2F4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD6A3DEB-4AEC-4843-9165-2FCF8F7ECD72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -978,8 +997,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7770090" cy="3971636"/>
+          <a:off x="785091" y="0"/>
+          <a:ext cx="10058400" cy="4155707"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1290,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1306,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
@@ -1317,7 +1336,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
@@ -1350,7 +1369,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
@@ -1361,7 +1380,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H12" s="24"/>
     </row>
@@ -1369,60 +1388,60 @@
       <c r="C13" s="19"/>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="2:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="340" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="D14" s="28"/>
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="2:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="31"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20" s="8"/>
     </row>
@@ -1431,28 +1450,28 @@
         <v>24</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" s="33"/>
     </row>
@@ -1517,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B24:G45"/>
+  <dimension ref="B24:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1568,10 +1587,10 @@
     </row>
     <row r="28" spans="2:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="40" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D28" s="39" t="s">
         <v>26</v>
@@ -1586,10 +1605,10 @@
     </row>
     <row r="29" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="40" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D29" s="39" t="s">
         <v>26</v>
@@ -1598,16 +1617,16 @@
         <v>25</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G29" s="22"/>
     </row>
     <row r="30" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="40" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D30" s="39"/>
       <c r="E30" s="41"/>
@@ -1616,10 +1635,10 @@
     </row>
     <row r="31" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="40" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D31" s="39"/>
       <c r="E31" s="41"/>
@@ -1628,10 +1647,10 @@
     </row>
     <row r="32" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="40" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D32" s="39"/>
       <c r="E32" s="41"/>
@@ -1640,10 +1659,10 @@
     </row>
     <row r="33" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="34" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D33" s="45" t="s">
         <v>26</v>
@@ -1658,19 +1677,19 @@
     </row>
     <row r="34" spans="2:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B34" s="40" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E34" s="41" t="s">
         <v>25</v>
       </c>
       <c r="F34" s="41" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G34" s="22"/>
     </row>
@@ -1684,7 +1703,7 @@
     </row>
     <row r="36" spans="2:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="42" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -1694,12 +1713,12 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
@@ -1708,7 +1727,7 @@
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="36" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="C42" s="36"/>
       <c r="D42" s="36"/>
@@ -1717,7 +1736,7 @@
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="36" t="s">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="C43" s="36"/>
       <c r="D43" s="36"/>
@@ -1726,7 +1745,7 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="36" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
       <c r="C44" s="36"/>
       <c r="D44" s="36"/>
@@ -1735,12 +1754,21 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
+        <v>48</v>
+      </c>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
       <c r="E45" s="38"/>
       <c r="F45" s="38"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B46" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1771,7 +1799,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2760,7 +2788,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3726,7 +3754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFD66BD-C60D-C14A-9E33-3479AADC1850}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -3739,21 +3767,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B2" s="52">
         <v>1</v>
@@ -3767,7 +3795,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B3" s="52">
         <v>1.49</v>
@@ -3781,7 +3809,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B4" s="52">
         <v>1.58</v>
@@ -3795,7 +3823,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B5" s="52">
         <v>1.57</v>
@@ -3809,7 +3837,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B6" s="52">
         <v>6.8000000000000005E-2</v>
@@ -3817,7 +3845,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="43" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B7" s="52">
         <v>3.9600000000000003E-2</v>
@@ -3825,7 +3853,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="51" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B8" s="54">
         <v>5.9799999999999999E-2</v>
@@ -3833,7 +3861,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="51" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B9" s="54">
         <v>3.9199999999999999E-3</v>
@@ -3847,7 +3875,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B10" s="54">
         <f>AVERAGE(C10:D10)</f>
@@ -3862,7 +3890,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B11" s="54">
         <f>AVERAGE(C11:D11)</f>
@@ -3877,7 +3905,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B12" s="52">
         <v>0.01</v>
@@ -3885,7 +3913,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="51" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B13" s="52">
         <v>0.34699999999999998</v>
@@ -3893,7 +3921,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B14" s="52">
         <v>0.185</v>
@@ -3901,7 +3929,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="51" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B15" s="52">
         <v>0.32500000000000001</v>
@@ -3909,7 +3937,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B16" s="52">
         <v>4.4999999999999998E-2</v>
@@ -3918,7 +3946,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="51" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B17" s="52">
         <v>0.35599999999999998</v>
@@ -3926,7 +3954,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="51" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B18" s="52">
         <v>0.245</v>
@@ -3934,7 +3962,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.2">
@@ -3957,27 +3985,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B2">
         <v>25</v>
@@ -3997,7 +4025,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B3">
         <v>25</v>
@@ -4017,7 +4045,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -4037,7 +4065,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B5">
         <v>25</v>
@@ -4057,7 +4085,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B6">
         <v>35</v>
@@ -4077,7 +4105,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B7">
         <v>45</v>
@@ -4097,7 +4125,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B8">
         <v>55</v>
@@ -4117,7 +4145,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B9">
         <v>25</v>
@@ -4137,7 +4165,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -4157,7 +4185,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B11">
         <v>45</v>
@@ -4177,7 +4205,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B12">
         <v>55</v>
@@ -4197,7 +4225,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B13">
         <v>25</v>
@@ -4217,7 +4245,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -4237,7 +4265,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B15">
         <v>45</v>
@@ -4257,7 +4285,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B16">
         <v>55</v>
@@ -4277,7 +4305,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -4292,7 +4320,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -4306,7 +4334,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4320,7 +4348,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -4334,7 +4362,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B21">
         <v>18</v>
@@ -4348,7 +4376,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B22">
         <v>18</v>
@@ -4362,7 +4390,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B23">
         <v>18</v>
@@ -4395,17 +4423,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C2" s="48" t="s">
         <v>17</v>
@@ -4413,79 +4441,79 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="47" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="47" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B5" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="47" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="47" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="47" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>